<commit_message>
added fail/exterior logic removed incomplete scenes
</commit_message>
<xml_diff>
--- a/Projects/CCUS/Validation/Data/Validation_Template_v1.0_.xlsx
+++ b/Projects/CCUS/Validation/Data/Validation_Template_v1.0_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">store_type</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cold Vault &amp; Coolers with Doors (Outside of Checkout Area), All Coolers At Checkout Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exterior Store Photo</t>
   </si>
 </sst>
 </file>
@@ -92,6 +98,7 @@
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,6 +153,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,18 +177,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="AI47" activeCellId="0" sqref="AI47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,6 +274,23 @@
       </c>
       <c r="E5" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>